<commit_message>
Updates to sprint 5 logs
</commit_message>
<xml_diff>
--- a/artifacts/sprint-5-logs.xlsx
+++ b/artifacts/sprint-5-logs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbens\dev\sosgame\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16EA852B-28D0-4C47-8677-D4AAC9974380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF99288-A4FC-4606-89E8-FBFEBAC77CB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7320" yWindow="45" windowWidth="21600" windowHeight="11190" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7320" yWindow="75" windowWidth="21600" windowHeight="11295" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="976" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1007" uniqueCount="455">
   <si>
     <t>ID</t>
   </si>
@@ -1433,6 +1433,67 @@
   </si>
   <si>
     <t>Testing of the SimpleGame class</t>
+  </si>
+  <si>
+    <t>Game record and replay</t>
+  </si>
+  <si>
+    <t>User replays a game when the previous game was not recorded</t>
+  </si>
+  <si>
+    <t>Given a SOS application outside of a game with the previous game not recorded, when the user replays the previous game, then the previous game will not be replayed</t>
+  </si>
+  <si>
+    <t>ReplayTest</t>
+  </si>
+  <si>
+    <t>ReplayTest.TestGetNextMoveEntry</t>
+  </si>
+  <si>
+    <t>Input: A file containing JSON data of move entries of a SOS game
+Output: The replay parses and steps through the correct move entries contained in the JSON data</t>
+  </si>
+  <si>
+    <t>Check the record button. Play through a simple or general game. Then start a new simple or general game, and try to replay the previous game while  playing the current game</t>
+  </si>
+  <si>
+    <t>Just after the application starts up, try to replay a game</t>
+  </si>
+  <si>
+    <t>The replay should not play because a game has not been played yet</t>
+  </si>
+  <si>
+    <t>The replay should not play because the user cannot play a replay while he is in the middle of a game</t>
+  </si>
+  <si>
+    <t>Do not check the record button. Play through a simple or general game. Then try to replay the previous game.</t>
+  </si>
+  <si>
+    <t>The replay should not play because the user did not check the record button before playing the previous game</t>
+  </si>
+  <si>
+    <t>ReplayTest.TestAtEnd</t>
+  </si>
+  <si>
+    <t>Replay.AtEnd</t>
+  </si>
+  <si>
+    <t>A Replay object that is not at the end of the replay</t>
+  </si>
+  <si>
+    <t>A Replay object that is at the end of the replay</t>
+  </si>
+  <si>
+    <t>Replay.cs</t>
+  </si>
+  <si>
+    <t>Replay class that associated with the playing of replays</t>
+  </si>
+  <si>
+    <t>ReplayTest.cs</t>
+  </si>
+  <si>
+    <t>Testing for the Replay class</t>
   </si>
 </sst>
 </file>
@@ -1494,7 +1555,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1541,6 +1602,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1550,21 +1618,301 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="62">
+  <dxfs count="67">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1761,6 +2109,9 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -1833,6 +2184,135 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1968,349 +2448,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2361,129 +2499,129 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F0B81098-1FDF-4645-B026-CB44129665D9}" name="Table1" displayName="Table1" ref="C4:G13" totalsRowShown="0" headerRowDxfId="61" dataDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F0B81098-1FDF-4645-B026-CB44129665D9}" name="Table1" displayName="Table1" ref="C4:G13" totalsRowShown="0" headerRowDxfId="66" dataDxfId="13">
   <autoFilter ref="C4:G13" xr:uid="{F0B81098-1FDF-4645-B026-CB44129665D9}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{2D6513DD-0333-4977-A611-BE7075C47F94}" name="ID" dataDxfId="48"/>
-    <tableColumn id="2" xr3:uid="{EA0F2575-5222-4342-B2A6-3C0DB80B27F6}" name="User Story Name" dataDxfId="47"/>
-    <tableColumn id="3" xr3:uid="{7B31B9E3-2E36-4F4A-87F2-E74CDAFDBBB4}" name="User Story Description" dataDxfId="46"/>
-    <tableColumn id="4" xr3:uid="{51BD8312-BA1E-4461-8AF6-E3CDCD58C707}" name="Priority" dataDxfId="45"/>
-    <tableColumn id="5" xr3:uid="{0D005556-7948-42BB-87C3-0F6B1D42DF95}" name="Estimated Effort (hours)" dataDxfId="44"/>
+    <tableColumn id="1" xr3:uid="{2D6513DD-0333-4977-A611-BE7075C47F94}" name="ID" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{EA0F2575-5222-4342-B2A6-3C0DB80B27F6}" name="User Story Name" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{7B31B9E3-2E36-4F4A-87F2-E74CDAFDBBB4}" name="User Story Description" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{51BD8312-BA1E-4461-8AF6-E3CDCD58C707}" name="Priority" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{0D005556-7948-42BB-87C3-0F6B1D42DF95}" name="Estimated Effort (hours)" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{412B69F0-FD73-4B7D-9BF6-3A0E4171D35B}" name="Table2" displayName="Table2" ref="B3:G37" totalsRowShown="0" dataDxfId="60">
-  <autoFilter ref="B3:G37" xr:uid="{412B69F0-FD73-4B7D-9BF6-3A0E4171D35B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{412B69F0-FD73-4B7D-9BF6-3A0E4171D35B}" name="Table2" displayName="Table2" ref="B3:G38" totalsRowShown="0" dataDxfId="65">
+  <autoFilter ref="B3:G38" xr:uid="{412B69F0-FD73-4B7D-9BF6-3A0E4171D35B}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{702A0B1D-F950-436C-AB51-03E5AFD84C94}" name="Story ID" dataDxfId="59"/>
-    <tableColumn id="2" xr3:uid="{B7C53018-BEB1-41CB-9DD0-4289A4847403}" name="Story Name" dataDxfId="58"/>
-    <tableColumn id="3" xr3:uid="{054381AB-35EE-48FB-9EE1-95AE48FEF0FA}" name="AC ID" dataDxfId="57"/>
-    <tableColumn id="7" xr3:uid="{CF360237-B28D-40DF-928D-FC30827FC043}" name="AC Name" dataDxfId="56"/>
-    <tableColumn id="4" xr3:uid="{E3125AC9-3CDD-40AA-A1CA-0204D9A63C5C}" name="Description of Acceptance Criterion" dataDxfId="55"/>
-    <tableColumn id="5" xr3:uid="{BD32E5D0-24DE-4E60-82C8-90E318E5EA1B}" name="Status" dataDxfId="54"/>
+    <tableColumn id="1" xr3:uid="{702A0B1D-F950-436C-AB51-03E5AFD84C94}" name="Story ID" dataDxfId="64"/>
+    <tableColumn id="2" xr3:uid="{B7C53018-BEB1-41CB-9DD0-4289A4847403}" name="Story Name" dataDxfId="63"/>
+    <tableColumn id="3" xr3:uid="{054381AB-35EE-48FB-9EE1-95AE48FEF0FA}" name="AC ID" dataDxfId="62"/>
+    <tableColumn id="7" xr3:uid="{CF360237-B28D-40DF-928D-FC30827FC043}" name="AC Name" dataDxfId="61"/>
+    <tableColumn id="4" xr3:uid="{E3125AC9-3CDD-40AA-A1CA-0204D9A63C5C}" name="Description of Acceptance Criterion" dataDxfId="60"/>
+    <tableColumn id="5" xr3:uid="{BD32E5D0-24DE-4E60-82C8-90E318E5EA1B}" name="Status" dataDxfId="59"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D36D6B9B-3977-42E1-9D3A-2AD19D09F63F}" name="Table3" displayName="Table3" ref="B4:E26" totalsRowCount="1">
-  <autoFilter ref="B4:E25" xr:uid="{D36D6B9B-3977-42E1-9D3A-2AD19D09F63F}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:E25">
-    <sortCondition ref="C5:C25"/>
-    <sortCondition descending="1" ref="E5:E25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D36D6B9B-3977-42E1-9D3A-2AD19D09F63F}" name="Table3" displayName="Table3" ref="B4:E28" totalsRowCount="1" dataDxfId="8">
+  <autoFilter ref="B4:E27" xr:uid="{D36D6B9B-3977-42E1-9D3A-2AD19D09F63F}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:E27">
+    <sortCondition ref="C5:C27"/>
+    <sortCondition descending="1" ref="E5:E27"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{DB279ACC-EE7F-4F69-9CDF-D6557C3D4B5F}" name="Source Code file Name"/>
-    <tableColumn id="2" xr3:uid="{AD6AFAE9-FED0-4CE4-8020-D0B3CA4EBBA2}" name="Production code or test code?"/>
-    <tableColumn id="4" xr3:uid="{FDFB077A-2AFB-452D-8B38-C052AFA8880B}" name="Notes" totalsRowLabel="Total"/>
-    <tableColumn id="3" xr3:uid="{9C1EC1B0-7F07-45F8-AACD-2593D2FB6FC3}" name="# Lines of Code" totalsRowFunction="sum"/>
+    <tableColumn id="1" xr3:uid="{DB279ACC-EE7F-4F69-9CDF-D6557C3D4B5F}" name="Source Code file Name" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{AD6AFAE9-FED0-4CE4-8020-D0B3CA4EBBA2}" name="Production code or test code?" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{FDFB077A-2AFB-452D-8B38-C052AFA8880B}" name="Notes" totalsRowLabel="Total" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{9C1EC1B0-7F07-45F8-AACD-2593D2FB6FC3}" name="# Lines of Code" totalsRowFunction="sum" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{8613F438-F257-4CB7-8127-41336443AD8E}" name="Table5" displayName="Table5" ref="B4:I35" totalsRowShown="0" headerRowDxfId="53" dataDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{8613F438-F257-4CB7-8127-41336443AD8E}" name="Table5" displayName="Table5" ref="B4:I35" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57">
   <autoFilter ref="B4:I35" xr:uid="{8613F438-F257-4CB7-8127-41336443AD8E}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{FA37DF55-838D-4C91-A069-B4ADFBB114FF}" name="Story ID" dataDxfId="42"/>
-    <tableColumn id="7" xr3:uid="{B29593B2-9E50-4429-B73E-C267894CE53F}" name="Story Name" dataDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{92144E97-78C1-4013-A5DC-A103AC987D08}" name="AC  ID" dataDxfId="40"/>
-    <tableColumn id="8" xr3:uid="{D34169B1-9605-4002-A5FC-55DBEC95591D}" name="AC Name" dataDxfId="39"/>
-    <tableColumn id="3" xr3:uid="{988A7BC5-9B7F-4EF4-9743-8B43044CA88C}" name="Classes" dataDxfId="38"/>
-    <tableColumn id="4" xr3:uid="{6962998B-BD75-44D2-8DE4-A3B7232E7D55}" name="Method Name(s) " dataDxfId="37"/>
-    <tableColumn id="5" xr3:uid="{8D2432C4-71E4-445C-BF93-B65E87280890}" name="Status" dataDxfId="36"/>
-    <tableColumn id="6" xr3:uid="{1E10CD18-6EE0-4C57-A597-745A6F075070}" name="Notes (optional)" dataDxfId="35"/>
+    <tableColumn id="1" xr3:uid="{FA37DF55-838D-4C91-A069-B4ADFBB114FF}" name="Story ID" dataDxfId="56"/>
+    <tableColumn id="7" xr3:uid="{B29593B2-9E50-4429-B73E-C267894CE53F}" name="Story Name" dataDxfId="55"/>
+    <tableColumn id="2" xr3:uid="{92144E97-78C1-4013-A5DC-A103AC987D08}" name="AC  ID" dataDxfId="54"/>
+    <tableColumn id="8" xr3:uid="{D34169B1-9605-4002-A5FC-55DBEC95591D}" name="AC Name" dataDxfId="53"/>
+    <tableColumn id="3" xr3:uid="{988A7BC5-9B7F-4EF4-9743-8B43044CA88C}" name="Classes" dataDxfId="52"/>
+    <tableColumn id="4" xr3:uid="{6962998B-BD75-44D2-8DE4-A3B7232E7D55}" name="Method Name(s) " dataDxfId="51"/>
+    <tableColumn id="5" xr3:uid="{8D2432C4-71E4-445C-BF93-B65E87280890}" name="Status" dataDxfId="50"/>
+    <tableColumn id="6" xr3:uid="{1E10CD18-6EE0-4C57-A597-745A6F075070}" name="Notes (optional)" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{AFC835DF-2809-4ADA-8933-35F8B41412B7}" name="Table6" displayName="Table6" ref="B3:H36" totalsRowShown="0" headerRowDxfId="52" dataDxfId="26">
-  <autoFilter ref="B3:H36" xr:uid="{AFC835DF-2809-4ADA-8933-35F8B41412B7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{AFC835DF-2809-4ADA-8933-35F8B41412B7}" name="Table6" displayName="Table6" ref="B3:H37" totalsRowShown="0" headerRowDxfId="48" dataDxfId="0">
+  <autoFilter ref="B3:H37" xr:uid="{AFC835DF-2809-4ADA-8933-35F8B41412B7}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{4D464094-4CAA-4F0A-8155-1005A5221EA7}" name="User Story ID" dataDxfId="33"/>
-    <tableColumn id="6" xr3:uid="{DFFD886B-21F5-4EE4-B1E5-B9C3CA981393}" name="User Story Name" dataDxfId="32"/>
-    <tableColumn id="2" xr3:uid="{588A5FF9-87E4-4232-A109-F00AE6EAB7C9}" name="AC ID" dataDxfId="31"/>
-    <tableColumn id="7" xr3:uid="{A723F0C9-F396-4182-A5DB-A36687ECC464}" name="AC Name" dataDxfId="30"/>
-    <tableColumn id="3" xr3:uid="{04A7B299-94AB-4FB7-8A08-822F463E676E}" name="Classes " dataDxfId="29"/>
-    <tableColumn id="4" xr3:uid="{263669AA-535C-4DA8-9C9A-A153A480F553}" name="Methods" dataDxfId="28"/>
-    <tableColumn id="5" xr3:uid="{9CFC3D83-A897-493C-A6B2-E4D0BA51E596}" name="Description" dataDxfId="27"/>
+    <tableColumn id="1" xr3:uid="{4D464094-4CAA-4F0A-8155-1005A5221EA7}" name="User Story ID" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{DFFD886B-21F5-4EE4-B1E5-B9C3CA981393}" name="User Story Name" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{588A5FF9-87E4-4232-A109-F00AE6EAB7C9}" name="AC ID" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{A723F0C9-F396-4182-A5DB-A36687ECC464}" name="AC Name" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{04A7B299-94AB-4FB7-8A08-822F463E676E}" name="Classes " dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{263669AA-535C-4DA8-9C9A-A153A480F553}" name="Methods" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{9CFC3D83-A897-493C-A6B2-E4D0BA51E596}" name="Description" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{A6E1AD56-1E7E-4845-A6DC-51274101CF0C}" name="Table69" displayName="Table69" ref="B3:G26" totalsRowShown="0" headerRowDxfId="51" dataDxfId="19">
-  <autoFilter ref="B3:G26" xr:uid="{AFC835DF-2809-4ADA-8933-35F8B41412B7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{A6E1AD56-1E7E-4845-A6DC-51274101CF0C}" name="Table69" displayName="Table69" ref="B3:G29" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
+  <autoFilter ref="B3:G29" xr:uid="{AFC835DF-2809-4ADA-8933-35F8B41412B7}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{301EF044-7DF2-4C9B-84A0-556EDC81E926}" name="User Story ID" dataDxfId="25"/>
-    <tableColumn id="6" xr3:uid="{C53176BB-A112-4BC9-B43C-A9B819FD40BE}" name="User Story Name" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{75701814-A8A2-49F2-9634-F7BCE794B67D}" name="AC ID" dataDxfId="23"/>
-    <tableColumn id="7" xr3:uid="{DB2FE0C2-4D4A-4FA4-AD4F-2F9ACE0E2772}" name="AC Name" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{5FE8A6D0-B4D1-471F-9956-459A848C1C0F}" name="Test Case Input" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{C8A349CF-C07B-44C4-B8D0-DD604B478305}" name="Test Oracle" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{301EF044-7DF2-4C9B-84A0-556EDC81E926}" name="User Story ID" dataDxfId="45"/>
+    <tableColumn id="6" xr3:uid="{C53176BB-A112-4BC9-B43C-A9B819FD40BE}" name="User Story Name" dataDxfId="44"/>
+    <tableColumn id="2" xr3:uid="{75701814-A8A2-49F2-9634-F7BCE794B67D}" name="AC ID" dataDxfId="43"/>
+    <tableColumn id="7" xr3:uid="{DB2FE0C2-4D4A-4FA4-AD4F-2F9ACE0E2772}" name="AC Name" dataDxfId="42"/>
+    <tableColumn id="4" xr3:uid="{5FE8A6D0-B4D1-471F-9956-459A848C1C0F}" name="Test Case Input" dataDxfId="41"/>
+    <tableColumn id="5" xr3:uid="{C8A349CF-C07B-44C4-B8D0-DD604B478305}" name="Test Oracle" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{0F699053-0EA0-422C-84BA-6343D3283560}" name="Table9" displayName="Table9" ref="B2:F28" totalsRowShown="0" headerRowDxfId="50" dataDxfId="13">
-  <autoFilter ref="B2:F28" xr:uid="{0F699053-0EA0-422C-84BA-6343D3283560}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{0F699053-0EA0-422C-84BA-6343D3283560}" name="Table9" displayName="Table9" ref="B2:F30" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
+  <autoFilter ref="B2:F30" xr:uid="{0F699053-0EA0-422C-84BA-6343D3283560}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{7EE5C09C-96A5-4FC0-A9B8-78BA2D61269E}" name="Number" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{B9AA6030-119E-443A-BB87-750EA97ECF8C}" name="Production Code Class.Method" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{49E194BC-903C-4C2D-AF6F-5DBC479ACEC9}" name="Test Code Class.Method" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{9D11DD5C-4AE4-4A5E-8750-0E12B5A106FA}" name="Test Input" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{8C3EBF53-C850-403C-B499-DB556E2F1A8B}" name="Expected Result" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{7EE5C09C-96A5-4FC0-A9B8-78BA2D61269E}" name="Number" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{B9AA6030-119E-443A-BB87-750EA97ECF8C}" name="Production Code Class.Method" dataDxfId="36"/>
+    <tableColumn id="5" xr3:uid="{49E194BC-903C-4C2D-AF6F-5DBC479ACEC9}" name="Test Code Class.Method" dataDxfId="35"/>
+    <tableColumn id="3" xr3:uid="{9D11DD5C-4AE4-4A5E-8750-0E12B5A106FA}" name="Test Input" dataDxfId="34"/>
+    <tableColumn id="4" xr3:uid="{8C3EBF53-C850-403C-B499-DB556E2F1A8B}" name="Expected Result" dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{69FD6488-0717-4BB3-A73F-84BDA7E946E5}" name="Table4" displayName="Table4" ref="A1:L513" totalsRowShown="0" headerRowDxfId="49" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{69FD6488-0717-4BB3-A73F-84BDA7E946E5}" name="Table4" displayName="Table4" ref="A1:L513" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
   <autoFilter ref="A1:L513" xr:uid="{69FD6488-0717-4BB3-A73F-84BDA7E946E5}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{4EEA4C52-25A8-4AC1-AB64-130F1061C5C0}" name="Control Name" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{528C3ED4-7A70-4ADC-A6E5-12A55306EB86}" name="Control A" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{5A820990-15C8-451A-AA81-A4FDEEF27F37}" name="Control B" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{90491295-6B5C-44D5-9DBA-7086E88AC0F9}" name="Control C" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{1C3B15D1-EB06-4A22-B868-6BE0E2AA4E0D}" name="Control D" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{EB1C9048-B008-4402-8AFC-D23757742E6F}" name="In Replay" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{B62C2260-705C-4FA8-AAD7-D8CDD79F071C}" name="In Game" dataDxfId="6"/>
-    <tableColumn id="12" xr3:uid="{7DBAE433-F5CB-4355-AA42-DF22721518A4}" name="Is Red Turn" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{E7051258-A7C3-4770-BF85-6A7E897040FA}" name="Is Blue Computer" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{672057EC-F845-40E7-A956-72F68FFFCD00}" name="Is Red Computer" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{43FEA681-4DBD-4D98-B67C-A034045E34F1}" name="Is Accessible" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{72EB1685-1373-450C-B014-35BFBA34CCA1}" name="Notes" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{4EEA4C52-25A8-4AC1-AB64-130F1061C5C0}" name="Control Name" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{528C3ED4-7A70-4ADC-A6E5-12A55306EB86}" name="Control A" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{5A820990-15C8-451A-AA81-A4FDEEF27F37}" name="Control B" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{90491295-6B5C-44D5-9DBA-7086E88AC0F9}" name="Control C" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{1C3B15D1-EB06-4A22-B868-6BE0E2AA4E0D}" name="Control D" dataDxfId="26"/>
+    <tableColumn id="6" xr3:uid="{EB1C9048-B008-4402-8AFC-D23757742E6F}" name="In Replay" dataDxfId="25"/>
+    <tableColumn id="7" xr3:uid="{B62C2260-705C-4FA8-AAD7-D8CDD79F071C}" name="In Game" dataDxfId="24"/>
+    <tableColumn id="12" xr3:uid="{7DBAE433-F5CB-4355-AA42-DF22721518A4}" name="Is Red Turn" dataDxfId="23"/>
+    <tableColumn id="8" xr3:uid="{E7051258-A7C3-4770-BF85-6A7E897040FA}" name="Is Blue Computer" dataDxfId="22"/>
+    <tableColumn id="9" xr3:uid="{672057EC-F845-40E7-A956-72F68FFFCD00}" name="Is Red Computer" dataDxfId="21"/>
+    <tableColumn id="10" xr3:uid="{43FEA681-4DBD-4D98-B67C-A034045E34F1}" name="Is Accessible" dataDxfId="20"/>
+    <tableColumn id="11" xr3:uid="{72EB1685-1373-450C-B014-35BFBA34CCA1}" name="Notes" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2755,7 +2893,7 @@
   <dimension ref="C2:G13"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2768,12 +2906,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="19" t="s">
         <v>335</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
     </row>
     <row r="4" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
@@ -2793,155 +2931,155 @@
       </c>
     </row>
     <row r="5" spans="3:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C5" s="19">
-        <v>1</v>
-      </c>
-      <c r="D5" s="20" t="s">
+      <c r="C5" s="22">
+        <v>1</v>
+      </c>
+      <c r="D5" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="19">
+      <c r="F5" s="22">
         <v>2</v>
       </c>
-      <c r="G5" s="19">
+      <c r="G5" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="3:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C6" s="19">
+      <c r="C6" s="22">
         <v>2</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="19">
+      <c r="F6" s="22">
         <v>3</v>
       </c>
-      <c r="G6" s="19">
+      <c r="G6" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="3:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C7" s="19">
+      <c r="C7" s="22">
         <v>3</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="19">
+      <c r="F7" s="22">
         <v>4</v>
       </c>
-      <c r="G7" s="19">
+      <c r="G7" s="22">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="3:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C8" s="19">
+      <c r="C8" s="22">
         <v>4</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="23" t="s">
         <v>400</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="19">
+      <c r="F8" s="22">
         <v>6</v>
       </c>
-      <c r="G8" s="19">
+      <c r="G8" s="22">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="3:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C9" s="19">
+      <c r="C9" s="22">
         <v>5</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="19">
+      <c r="F9" s="22">
         <v>7</v>
       </c>
-      <c r="G9" s="19">
+      <c r="G9" s="22">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="3:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C10" s="19">
+      <c r="C10" s="22">
         <v>6</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="19">
+      <c r="F10" s="22">
         <v>8</v>
       </c>
-      <c r="G10" s="19">
+      <c r="G10" s="22">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="3:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C11" s="19">
+      <c r="C11" s="14">
         <v>7</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="19">
+      <c r="F11" s="14">
         <v>8</v>
       </c>
-      <c r="G11" s="19">
+      <c r="G11" s="14">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="3:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C12" s="19">
+      <c r="C12" s="22">
         <v>8</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="19">
+      <c r="F12" s="22">
         <v>5</v>
       </c>
-      <c r="G12" s="19">
+      <c r="G12" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="3:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C13" s="14">
+      <c r="C13" s="22">
         <v>9</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="23" t="s">
         <v>399</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="24" t="s">
         <v>401</v>
       </c>
-      <c r="F13" s="14">
+      <c r="F13" s="22">
         <v>9</v>
       </c>
-      <c r="G13" s="14">
+      <c r="G13" s="22">
         <v>3</v>
       </c>
     </row>
@@ -2959,10 +3097,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DCE3E03-8907-42B0-9BAE-1522C8D2D080}">
-  <dimension ref="B2:H48"/>
+  <dimension ref="B2:H49"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33:E37"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29:E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2976,15 +3114,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -3242,7 +3380,9 @@
       <c r="F17" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="G17" s="3"/>
+      <c r="G17" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="18" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B18" s="3"/>
@@ -3256,10 +3396,12 @@
       <c r="F18" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="G18" s="3"/>
+      <c r="G18" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="19" spans="2:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="B19" s="20">
+      <c r="B19" s="16">
         <v>5</v>
       </c>
       <c r="C19" s="5" t="s">
@@ -3274,12 +3416,12 @@
       <c r="F19" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="G19" s="20" t="s">
+      <c r="G19" s="16" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="B20" s="20"/>
+      <c r="B20" s="16"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5">
         <v>5.2</v>
@@ -3290,12 +3432,12 @@
       <c r="F20" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="G20" s="20" t="s">
+      <c r="G20" s="16" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="B21" s="20"/>
+      <c r="B21" s="16"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5">
         <v>5.3</v>
@@ -3306,12 +3448,12 @@
       <c r="F21" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="G21" s="20" t="s">
+      <c r="G21" s="16" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="B22" s="20">
+      <c r="B22" s="16">
         <v>6</v>
       </c>
       <c r="C22" s="5" t="s">
@@ -3326,12 +3468,12 @@
       <c r="F22" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="G22" s="20" t="s">
+      <c r="G22" s="16" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="B23" s="20"/>
+      <c r="B23" s="16"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5">
         <v>6.2</v>
@@ -3342,12 +3484,12 @@
       <c r="F23" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="G23" s="20" t="s">
+      <c r="G23" s="16" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="B24" s="20"/>
+      <c r="B24" s="16"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5">
         <v>6.3</v>
@@ -3358,12 +3500,12 @@
       <c r="F24" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="G24" s="20" t="s">
+      <c r="G24" s="16" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="25" spans="2:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="B25" s="20"/>
+      <c r="B25" s="16"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5">
         <v>6.4</v>
@@ -3374,93 +3516,91 @@
       <c r="F25" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="G25" s="20" t="s">
+      <c r="G25" s="16" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="26" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B26" s="3">
+      <c r="B26" s="12">
         <v>7</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26" s="4">
+      <c r="C26" s="13" t="s">
+        <v>435</v>
+      </c>
+      <c r="D26" s="13">
         <v>7.1</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="F26" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="G26" s="3" t="s">
+      <c r="G26" s="12" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="27" spans="2:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="B27" s="3"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4">
+      <c r="B27" s="12"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13">
         <v>7.2</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E27" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="F27" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="G27" s="3" t="s">
+      <c r="G27" s="12" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="28" spans="2:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="B28" s="3"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4">
+      <c r="B28" s="12"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13">
         <v>7.3</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E28" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="F28" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="G28" s="3" t="s">
+      <c r="G28" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B29" s="3">
+    <row r="29" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B29" s="12"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13">
+        <v>7.4</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>436</v>
+      </c>
+      <c r="F29" s="13" t="s">
+        <v>437</v>
+      </c>
+      <c r="G29" s="12"/>
+    </row>
+    <row r="30" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B30" s="3">
         <v>8</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C30" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D29" s="4">
+      <c r="D30" s="4">
         <v>8.1</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E30" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F29" s="4" t="s">
+      <c r="F30" s="4" t="s">
         <v>73</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B30" s="3"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>76</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>17</v>
@@ -3470,13 +3610,13 @@
       <c r="B31" s="3"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4">
-        <v>8.3000000000000007</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>76</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>17</v>
@@ -3486,109 +3626,117 @@
       <c r="B32" s="3"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4">
-        <v>8.4</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>253</v>
+        <v>75</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>254</v>
+        <v>77</v>
       </c>
       <c r="G32" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="2:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="B33" s="12">
+    <row r="33" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B33" s="3"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4">
+        <v>8.4</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B34" s="23">
         <v>9</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C34" s="24" t="s">
         <v>399</v>
       </c>
-      <c r="D33" s="13">
+      <c r="D34" s="24">
         <v>8.1</v>
       </c>
-      <c r="E33" s="13" t="s">
+      <c r="E34" s="24" t="s">
         <v>405</v>
       </c>
-      <c r="F33" s="13" t="s">
+      <c r="F34" s="24" t="s">
         <v>404</v>
       </c>
-      <c r="G33" s="12" t="s">
+      <c r="G34" s="23" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="2:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="B34" s="12"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13">
+    <row r="35" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="B35" s="23"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="24">
         <v>8.1999999999999993</v>
       </c>
-      <c r="E34" s="13" t="s">
+      <c r="E35" s="24" t="s">
         <v>406</v>
       </c>
-      <c r="F34" s="13" t="s">
+      <c r="F35" s="24" t="s">
         <v>408</v>
       </c>
-      <c r="G34" s="12" t="s">
+      <c r="G35" s="23" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="2:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="B35" s="12"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13">
+    <row r="36" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B36" s="23"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="24">
         <v>8.3000000000000007</v>
       </c>
-      <c r="E35" s="13" t="s">
+      <c r="E36" s="24" t="s">
         <v>402</v>
       </c>
-      <c r="F35" s="13" t="s">
+      <c r="F36" s="24" t="s">
         <v>409</v>
       </c>
-      <c r="G35" s="12" t="s">
+      <c r="G36" s="23" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="2:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="B36" s="12"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13">
+    <row r="37" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B37" s="23"/>
+      <c r="C37" s="24"/>
+      <c r="D37" s="24">
         <v>8.4</v>
       </c>
-      <c r="E36" s="13" t="s">
+      <c r="E37" s="24" t="s">
         <v>403</v>
       </c>
-      <c r="F36" s="13" t="s">
+      <c r="F37" s="24" t="s">
         <v>410</v>
       </c>
-      <c r="G36" s="12" t="s">
+      <c r="G37" s="23" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="2:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="B37" s="12"/>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13">
+    <row r="38" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B38" s="23"/>
+      <c r="C38" s="24"/>
+      <c r="D38" s="24">
         <v>8.5</v>
       </c>
-      <c r="E37" s="13" t="s">
+      <c r="E38" s="24" t="s">
         <v>407</v>
       </c>
-      <c r="F37" s="13" t="s">
+      <c r="F38" s="24" t="s">
         <v>411</v>
       </c>
-      <c r="G37" s="12" t="s">
+      <c r="G38" s="23" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="3"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B39" s="3"/>
@@ -3669,6 +3817,14 @@
       <c r="E48" s="4"/>
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B49" s="3"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3684,10 +3840,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1EAF2C1-6E6A-4763-B1B8-87DF226FCFDA}">
-  <dimension ref="B4:E26"/>
+  <dimension ref="B4:E28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3712,306 +3868,334 @@
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="25" t="s">
         <v>158</v>
       </c>
-      <c r="E5" s="22">
-        <v>1064</v>
+      <c r="E5" s="25">
+        <v>1073</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="18" t="s">
         <v>144</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="18" t="s">
         <v>156</v>
       </c>
-      <c r="E6" s="22">
-        <v>501</v>
+      <c r="E6" s="18">
+        <v>556</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="B7" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="25" t="s">
         <v>155</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="25">
         <v>215</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="E8" s="18">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C9" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D9" s="25" t="s">
         <v>159</v>
       </c>
-      <c r="E8" s="22">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="E9" s="25">
         <v>153</v>
       </c>
-      <c r="C9" t="s">
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="C10" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="D9" t="s">
-        <v>165</v>
-      </c>
-      <c r="E9">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="22" t="s">
-        <v>146</v>
-      </c>
-      <c r="C10" s="22" t="s">
+      <c r="D10" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="E10" s="25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="25" t="s">
+        <v>150</v>
+      </c>
+      <c r="C11" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="22" t="s">
-        <v>157</v>
-      </c>
-      <c r="E10" s="22">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>150</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="D11" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="E11" s="25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="25" t="s">
+        <v>151</v>
+      </c>
+      <c r="C12" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="D11" t="s">
-        <v>163</v>
-      </c>
-      <c r="E11">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>151</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="D12" s="25" t="s">
+        <v>164</v>
+      </c>
+      <c r="E12" s="25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="C13" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="D12" t="s">
-        <v>164</v>
-      </c>
-      <c r="E12">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>148</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="D13" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="E13" s="25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="C14" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="D13" t="s">
-        <v>160</v>
-      </c>
-      <c r="E13">
+      <c r="D14" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="E14" s="25">
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>154</v>
-      </c>
-      <c r="C14" t="s">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="25" t="s">
+        <v>152</v>
+      </c>
+      <c r="C15" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="D14" t="s">
-        <v>166</v>
-      </c>
-      <c r="E14">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="C15" s="22" t="s">
+      <c r="D15" s="25" t="s">
+        <v>161</v>
+      </c>
+      <c r="E15" s="25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="18" t="s">
+        <v>451</v>
+      </c>
+      <c r="C16" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="22" t="s">
+      <c r="D16" s="18" t="s">
+        <v>452</v>
+      </c>
+      <c r="E16" s="18">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>162</v>
+      </c>
+      <c r="E17" s="25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="25" t="s">
+        <v>191</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>263</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>192</v>
+      </c>
+      <c r="E18" s="25">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="25" t="s">
+        <v>431</v>
+      </c>
+      <c r="C19" s="25" t="s">
+        <v>263</v>
+      </c>
+      <c r="D19" s="25" t="s">
+        <v>432</v>
+      </c>
+      <c r="E19" s="25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="25" t="s">
+        <v>323</v>
+      </c>
+      <c r="C20" s="25" t="s">
+        <v>263</v>
+      </c>
+      <c r="D20" s="25" t="s">
+        <v>324</v>
+      </c>
+      <c r="E20" s="25">
         <v>161</v>
       </c>
-      <c r="E15" s="22">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>149</v>
-      </c>
-      <c r="C16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" t="s">
-        <v>162</v>
-      </c>
-      <c r="E16">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>191</v>
-      </c>
-      <c r="C17" t="s">
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="25" t="s">
+        <v>433</v>
+      </c>
+      <c r="C21" s="25" t="s">
         <v>263</v>
       </c>
-      <c r="D17" t="s">
-        <v>192</v>
-      </c>
-      <c r="E17">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>431</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="D21" s="25" t="s">
+        <v>434</v>
+      </c>
+      <c r="E21" s="25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="25" t="s">
+        <v>322</v>
+      </c>
+      <c r="C22" s="25" t="s">
         <v>263</v>
       </c>
-      <c r="D18" t="s">
-        <v>432</v>
-      </c>
-      <c r="E18">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="22" t="s">
-        <v>323</v>
-      </c>
-      <c r="C19" s="22" t="s">
+      <c r="D22" s="25" t="s">
+        <v>266</v>
+      </c>
+      <c r="E22" s="25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="25" t="s">
+        <v>265</v>
+      </c>
+      <c r="C23" s="25" t="s">
         <v>263</v>
       </c>
-      <c r="D19" s="22" t="s">
-        <v>324</v>
-      </c>
-      <c r="E19" s="22">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>433</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="D23" s="25" t="s">
+        <v>268</v>
+      </c>
+      <c r="E23" s="25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="18" t="s">
+        <v>453</v>
+      </c>
+      <c r="C24" s="18" t="s">
         <v>263</v>
       </c>
-      <c r="D20" t="s">
-        <v>434</v>
-      </c>
-      <c r="E20">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>322</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="D24" s="18" t="s">
+        <v>454</v>
+      </c>
+      <c r="E24" s="18">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="25" t="s">
+        <v>264</v>
+      </c>
+      <c r="C25" s="25" t="s">
         <v>263</v>
       </c>
-      <c r="D21" t="s">
-        <v>266</v>
-      </c>
-      <c r="E21">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>265</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="D25" s="25" t="s">
+        <v>267</v>
+      </c>
+      <c r="E25" s="25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="25" t="s">
+        <v>327</v>
+      </c>
+      <c r="C26" s="25" t="s">
         <v>263</v>
       </c>
-      <c r="D22" t="s">
-        <v>268</v>
-      </c>
-      <c r="E22">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>264</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="D26" s="25" t="s">
+        <v>328</v>
+      </c>
+      <c r="E26" s="25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="25" t="s">
+        <v>325</v>
+      </c>
+      <c r="C27" s="25" t="s">
         <v>263</v>
       </c>
-      <c r="D23" t="s">
-        <v>267</v>
-      </c>
-      <c r="E23">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>327</v>
-      </c>
-      <c r="C24" t="s">
-        <v>263</v>
-      </c>
-      <c r="D24" t="s">
-        <v>328</v>
-      </c>
-      <c r="E24">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>325</v>
-      </c>
-      <c r="C25" t="s">
-        <v>263</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="D27" s="25" t="s">
         <v>326</v>
       </c>
-      <c r="E25">
+      <c r="E27" s="25">
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D26" t="s">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
         <v>27</v>
       </c>
-      <c r="E26">
+      <c r="E28">
         <f>SUBTOTAL(109,Table3['# Lines of Code])</f>
-        <v>3806</v>
+        <v>4046</v>
       </c>
     </row>
   </sheetData>
@@ -4026,8 +4210,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BDFD0F4-363F-419F-B294-A046D2B416F4}">
   <dimension ref="B4:I35"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView topLeftCell="A21" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4071,7 +4255,7 @@
       </c>
     </row>
     <row r="5" spans="2:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="B5" s="21">
+      <c r="B5" s="17">
         <v>1</v>
       </c>
       <c r="C5" s="9" t="s">
@@ -4089,7 +4273,7 @@
       <c r="G5" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="H5" s="21" t="s">
+      <c r="H5" s="17" t="s">
         <v>172</v>
       </c>
       <c r="I5" s="9" t="s">
@@ -4097,7 +4281,7 @@
       </c>
     </row>
     <row r="6" spans="2:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="B6" s="21"/>
+      <c r="B6" s="17"/>
       <c r="C6" s="9"/>
       <c r="D6" s="9">
         <v>1.2</v>
@@ -4111,7 +4295,7 @@
       <c r="G6" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="H6" s="21" t="s">
+      <c r="H6" s="17" t="s">
         <v>172</v>
       </c>
       <c r="I6" s="9" t="s">
@@ -4119,7 +4303,7 @@
       </c>
     </row>
     <row r="7" spans="2:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="B7" s="21"/>
+      <c r="B7" s="17"/>
       <c r="C7" s="9"/>
       <c r="D7" s="9">
         <v>1.3</v>
@@ -4133,7 +4317,7 @@
       <c r="G7" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="H7" s="21" t="s">
+      <c r="H7" s="17" t="s">
         <v>172</v>
       </c>
       <c r="I7" s="9" t="s">
@@ -4141,7 +4325,7 @@
       </c>
     </row>
     <row r="8" spans="2:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="B8" s="21"/>
+      <c r="B8" s="17"/>
       <c r="C8" s="9"/>
       <c r="D8" s="9">
         <v>1.4</v>
@@ -4155,7 +4339,7 @@
       <c r="G8" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="H8" s="21" t="s">
+      <c r="H8" s="17" t="s">
         <v>172</v>
       </c>
       <c r="I8" s="9" t="s">
@@ -4163,7 +4347,7 @@
       </c>
     </row>
     <row r="9" spans="2:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="B9" s="20">
+      <c r="B9" s="16">
         <v>2</v>
       </c>
       <c r="C9" s="5" t="s">
@@ -4181,7 +4365,7 @@
       <c r="G9" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="H9" s="21" t="s">
+      <c r="H9" s="17" t="s">
         <v>172</v>
       </c>
       <c r="I9" s="9" t="s">
@@ -4189,7 +4373,7 @@
       </c>
     </row>
     <row r="10" spans="2:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B10" s="20"/>
+      <c r="B10" s="16"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5">
         <v>2.2000000000000002</v>
@@ -4203,7 +4387,7 @@
       <c r="G10" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="H10" s="21" t="s">
+      <c r="H10" s="17" t="s">
         <v>172</v>
       </c>
       <c r="I10" s="9" t="s">
@@ -4211,7 +4395,7 @@
       </c>
     </row>
     <row r="11" spans="2:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="B11" s="20"/>
+      <c r="B11" s="16"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5">
         <v>2.2999999999999998</v>
@@ -4225,7 +4409,7 @@
       <c r="G11" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="H11" s="21" t="s">
+      <c r="H11" s="17" t="s">
         <v>172</v>
       </c>
       <c r="I11" s="9" t="s">
@@ -4233,7 +4417,7 @@
       </c>
     </row>
     <row r="12" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B12" s="20"/>
+      <c r="B12" s="16"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5">
         <v>2.4</v>
@@ -4247,7 +4431,7 @@
       <c r="G12" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="H12" s="21" t="s">
+      <c r="H12" s="17" t="s">
         <v>172</v>
       </c>
       <c r="I12" s="9" t="s">
@@ -4255,7 +4439,7 @@
       </c>
     </row>
     <row r="13" spans="2:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="B13" s="20">
+      <c r="B13" s="16">
         <v>3</v>
       </c>
       <c r="C13" s="5" t="s">
@@ -4273,7 +4457,7 @@
       <c r="G13" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="H13" s="21" t="s">
+      <c r="H13" s="17" t="s">
         <v>172</v>
       </c>
       <c r="I13" s="9" t="s">
@@ -4281,7 +4465,7 @@
       </c>
     </row>
     <row r="14" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="20"/>
+      <c r="B14" s="16"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5">
         <v>3.2</v>
@@ -4295,7 +4479,7 @@
       <c r="G14" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="H14" s="21" t="s">
+      <c r="H14" s="17" t="s">
         <v>172</v>
       </c>
       <c r="I14" s="9" t="s">
@@ -4303,7 +4487,7 @@
       </c>
     </row>
     <row r="15" spans="2:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="B15" s="20">
+      <c r="B15" s="16">
         <v>4</v>
       </c>
       <c r="C15" s="5" t="s">
@@ -4321,7 +4505,7 @@
       <c r="G15" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="H15" s="21" t="s">
+      <c r="H15" s="17" t="s">
         <v>172</v>
       </c>
       <c r="I15" s="9" t="s">
@@ -4329,7 +4513,7 @@
       </c>
     </row>
     <row r="16" spans="2:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B16" s="20"/>
+      <c r="B16" s="16"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5">
         <v>4.2</v>
@@ -4343,7 +4527,7 @@
       <c r="G16" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="H16" s="21" t="s">
+      <c r="H16" s="17" t="s">
         <v>172</v>
       </c>
       <c r="I16" s="9" t="s">
@@ -4351,7 +4535,7 @@
       </c>
     </row>
     <row r="17" spans="2:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B17" s="20"/>
+      <c r="B17" s="16"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5">
         <v>4.3</v>
@@ -4365,7 +4549,7 @@
       <c r="G17" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="H17" s="21" t="s">
+      <c r="H17" s="17" t="s">
         <v>172</v>
       </c>
       <c r="I17" s="9" t="s">
@@ -4373,7 +4557,7 @@
       </c>
     </row>
     <row r="18" spans="2:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B18" s="20"/>
+      <c r="B18" s="16"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5">
         <v>4.4000000000000004</v>
@@ -4387,7 +4571,7 @@
       <c r="G18" s="9" t="s">
         <v>233</v>
       </c>
-      <c r="H18" s="21" t="s">
+      <c r="H18" s="17" t="s">
         <v>172</v>
       </c>
       <c r="I18" s="9" t="s">
@@ -4395,8 +4579,8 @@
       </c>
     </row>
     <row r="19" spans="2:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
       <c r="D19" s="5">
         <v>4.5</v>
       </c>
@@ -4409,7 +4593,7 @@
       <c r="G19" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="H19" s="21" t="s">
+      <c r="H19" s="17" t="s">
         <v>172</v>
       </c>
       <c r="I19" s="9" t="s">
@@ -4417,7 +4601,7 @@
       </c>
     </row>
     <row r="20" spans="2:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="B20" s="21">
+      <c r="B20" s="17">
         <v>5</v>
       </c>
       <c r="C20" s="9" t="s">
@@ -4435,7 +4619,7 @@
       <c r="G20" s="9" t="s">
         <v>331</v>
       </c>
-      <c r="H20" s="21" t="s">
+      <c r="H20" s="17" t="s">
         <v>172</v>
       </c>
       <c r="I20" s="9" t="s">
@@ -4443,8 +4627,8 @@
       </c>
     </row>
     <row r="21" spans="2:9" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
       <c r="D21" s="9">
         <v>5.2</v>
       </c>
@@ -4457,7 +4641,7 @@
       <c r="G21" s="9" t="s">
         <v>331</v>
       </c>
-      <c r="H21" s="21" t="s">
+      <c r="H21" s="17" t="s">
         <v>172</v>
       </c>
       <c r="I21" s="9" t="s">
@@ -4465,8 +4649,8 @@
       </c>
     </row>
     <row r="22" spans="2:9" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="21"/>
-      <c r="C22" s="21"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
       <c r="D22" s="9">
         <v>5.3</v>
       </c>
@@ -4479,7 +4663,7 @@
       <c r="G22" s="9" t="s">
         <v>331</v>
       </c>
-      <c r="H22" s="21" t="s">
+      <c r="H22" s="17" t="s">
         <v>172</v>
       </c>
       <c r="I22" s="9" t="s">
@@ -4487,7 +4671,7 @@
       </c>
     </row>
     <row r="23" spans="2:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="B23" s="21">
+      <c r="B23" s="17">
         <v>6</v>
       </c>
       <c r="C23" s="9" t="s">
@@ -4505,7 +4689,7 @@
       <c r="G23" s="9" t="s">
         <v>348</v>
       </c>
-      <c r="H23" s="21" t="s">
+      <c r="H23" s="17" t="s">
         <v>172</v>
       </c>
       <c r="I23" s="9" t="s">
@@ -4513,8 +4697,8 @@
       </c>
     </row>
     <row r="24" spans="2:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="B24" s="21"/>
-      <c r="C24" s="21"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
       <c r="D24" s="9">
         <v>6.2</v>
       </c>
@@ -4527,7 +4711,7 @@
       <c r="G24" s="9" t="s">
         <v>351</v>
       </c>
-      <c r="H24" s="21" t="s">
+      <c r="H24" s="17" t="s">
         <v>172</v>
       </c>
       <c r="I24" s="9" t="s">
@@ -4535,8 +4719,8 @@
       </c>
     </row>
     <row r="25" spans="2:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
       <c r="D25" s="9">
         <v>6.3</v>
       </c>
@@ -4549,7 +4733,7 @@
       <c r="G25" s="9" t="s">
         <v>348</v>
       </c>
-      <c r="H25" s="21" t="s">
+      <c r="H25" s="17" t="s">
         <v>172</v>
       </c>
       <c r="I25" s="9" t="s">
@@ -4557,8 +4741,8 @@
       </c>
     </row>
     <row r="26" spans="2:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
       <c r="D26" s="9">
         <v>6.4</v>
       </c>
@@ -4571,7 +4755,7 @@
       <c r="G26" s="9" t="s">
         <v>348</v>
       </c>
-      <c r="H26" s="21" t="s">
+      <c r="H26" s="17" t="s">
         <v>172</v>
       </c>
       <c r="I26" s="9" t="s">
@@ -4579,7 +4763,7 @@
       </c>
     </row>
     <row r="27" spans="2:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="B27" s="20">
+      <c r="B27" s="16">
         <v>8</v>
       </c>
       <c r="C27" s="5" t="s">
@@ -4597,7 +4781,7 @@
       <c r="G27" s="9" t="s">
         <v>249</v>
       </c>
-      <c r="H27" s="21" t="s">
+      <c r="H27" s="17" t="s">
         <v>172</v>
       </c>
       <c r="I27" s="9" t="s">
@@ -4605,7 +4789,7 @@
       </c>
     </row>
     <row r="28" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B28" s="20"/>
+      <c r="B28" s="16"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5">
         <v>8.1999999999999993</v>
@@ -4619,7 +4803,7 @@
       <c r="G28" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="H28" s="21" t="s">
+      <c r="H28" s="17" t="s">
         <v>172</v>
       </c>
       <c r="I28" s="9" t="s">
@@ -4627,7 +4811,7 @@
       </c>
     </row>
     <row r="29" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B29" s="20"/>
+      <c r="B29" s="16"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5">
         <v>8.3000000000000007</v>
@@ -4641,7 +4825,7 @@
       <c r="G29" s="9" t="s">
         <v>249</v>
       </c>
-      <c r="H29" s="21" t="s">
+      <c r="H29" s="17" t="s">
         <v>172</v>
       </c>
       <c r="I29" s="9" t="s">
@@ -4649,7 +4833,7 @@
       </c>
     </row>
     <row r="30" spans="2:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B30" s="21"/>
+      <c r="B30" s="17"/>
       <c r="C30" s="9"/>
       <c r="D30" s="9">
         <v>8.4</v>
@@ -4663,7 +4847,7 @@
       <c r="G30" s="9" t="s">
         <v>255</v>
       </c>
-      <c r="H30" s="21" t="s">
+      <c r="H30" s="17" t="s">
         <v>172</v>
       </c>
       <c r="I30" s="9" t="s">
@@ -4671,116 +4855,116 @@
       </c>
     </row>
     <row r="31" spans="2:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="B31" s="10">
+      <c r="B31" s="17">
         <v>9</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="9" t="s">
         <v>399</v>
       </c>
-      <c r="D31" s="11">
+      <c r="D31" s="9">
         <v>8.1</v>
       </c>
-      <c r="E31" s="11" t="s">
+      <c r="E31" s="9" t="s">
         <v>405</v>
       </c>
-      <c r="F31" s="11" t="s">
+      <c r="F31" s="9" t="s">
         <v>423</v>
       </c>
-      <c r="G31" s="11" t="s">
+      <c r="G31" s="9" t="s">
         <v>424</v>
       </c>
-      <c r="H31" s="10" t="s">
+      <c r="H31" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="I31" s="11" t="s">
+      <c r="I31" s="9" t="s">
         <v>427</v>
       </c>
     </row>
     <row r="32" spans="2:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="B32" s="10"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11">
+      <c r="B32" s="17"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9">
         <v>8.1999999999999993</v>
       </c>
-      <c r="E32" s="11" t="s">
+      <c r="E32" s="9" t="s">
         <v>406</v>
       </c>
-      <c r="F32" s="11" t="s">
+      <c r="F32" s="9" t="s">
         <v>423</v>
       </c>
-      <c r="G32" s="11" t="s">
+      <c r="G32" s="9" t="s">
         <v>424</v>
       </c>
-      <c r="H32" s="10" t="s">
+      <c r="H32" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="I32" s="11" t="s">
+      <c r="I32" s="9" t="s">
         <v>427</v>
       </c>
     </row>
     <row r="33" spans="2:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="B33" s="10"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11">
+      <c r="B33" s="17"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9">
         <v>8.3000000000000007</v>
       </c>
-      <c r="E33" s="11" t="s">
+      <c r="E33" s="9" t="s">
         <v>402</v>
       </c>
-      <c r="F33" s="11" t="s">
+      <c r="F33" s="9" t="s">
         <v>423</v>
       </c>
-      <c r="G33" s="11" t="s">
+      <c r="G33" s="9" t="s">
         <v>425</v>
       </c>
-      <c r="H33" s="10" t="s">
+      <c r="H33" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="I33" s="11" t="s">
+      <c r="I33" s="9" t="s">
         <v>428</v>
       </c>
     </row>
     <row r="34" spans="2:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="B34" s="10"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11">
+      <c r="B34" s="17"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9">
         <v>8.4</v>
       </c>
-      <c r="E34" s="11" t="s">
+      <c r="E34" s="9" t="s">
         <v>403</v>
       </c>
-      <c r="F34" s="11" t="s">
+      <c r="F34" s="9" t="s">
         <v>423</v>
       </c>
-      <c r="G34" s="11" t="s">
+      <c r="G34" s="9" t="s">
         <v>426</v>
       </c>
-      <c r="H34" s="10" t="s">
+      <c r="H34" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="I34" s="11" t="s">
+      <c r="I34" s="9" t="s">
         <v>429</v>
       </c>
     </row>
     <row r="35" spans="2:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B35" s="10"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11">
+      <c r="B35" s="17"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9">
         <v>8.5</v>
       </c>
-      <c r="E35" s="11" t="s">
+      <c r="E35" s="9" t="s">
         <v>407</v>
       </c>
-      <c r="F35" s="11" t="s">
+      <c r="F35" s="9" t="s">
         <v>423</v>
       </c>
-      <c r="G35" s="11" t="s">
+      <c r="G35" s="9" t="s">
         <v>426</v>
       </c>
-      <c r="H35" s="10" t="s">
+      <c r="H35" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="I35" s="11" t="s">
+      <c r="I35" s="9" t="s">
         <v>430</v>
       </c>
     </row>
@@ -4794,10 +4978,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11A737DB-AD5B-4BBA-89D3-5F2C1DDAB7EB}">
-  <dimension ref="B3:H36"/>
+  <dimension ref="B3:H37"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView topLeftCell="A24" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4932,16 +5116,16 @@
       </c>
     </row>
     <row r="9" spans="2:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="B9" s="5">
+      <c r="B9" s="9">
         <v>2</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="9">
         <v>2.1</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="9" t="s">
         <v>43</v>
       </c>
       <c r="F9" s="9" t="s">
@@ -4955,12 +5139,12 @@
       </c>
     </row>
     <row r="10" spans="2:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5">
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9">
         <v>2.2000000000000002</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="9" t="s">
         <v>45</v>
       </c>
       <c r="F10" s="9" t="s">
@@ -4974,12 +5158,12 @@
       </c>
     </row>
     <row r="11" spans="2:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5">
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9">
         <v>2.2999999999999998</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="9" t="s">
         <v>47</v>
       </c>
       <c r="F11" s="9" t="s">
@@ -4993,12 +5177,12 @@
       </c>
     </row>
     <row r="12" spans="2:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5">
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9">
         <v>2.4</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="9" t="s">
         <v>50</v>
       </c>
       <c r="F12" s="9" t="s">
@@ -5027,16 +5211,16 @@
       </c>
     </row>
     <row r="14" spans="2:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="B14" s="5">
+      <c r="B14" s="9">
         <v>3</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="9">
         <v>3.1</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="9" t="s">
         <v>51</v>
       </c>
       <c r="F14" s="9" t="s">
@@ -5050,12 +5234,12 @@
       </c>
     </row>
     <row r="15" spans="2:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5">
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9">
         <v>3.2</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="9" t="s">
         <v>52</v>
       </c>
       <c r="F15" s="9" t="s">
@@ -5069,16 +5253,16 @@
       </c>
     </row>
     <row r="16" spans="2:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="B16" s="5">
+      <c r="B16" s="9">
         <v>4</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="9">
         <v>4.0999999999999996</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="9" t="s">
         <v>134</v>
       </c>
       <c r="F16" s="9" t="s">
@@ -5092,12 +5276,12 @@
       </c>
     </row>
     <row r="17" spans="2:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5">
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9">
         <v>4.2</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="9" t="s">
         <v>133</v>
       </c>
       <c r="F17" s="9" t="s">
@@ -5111,12 +5295,12 @@
       </c>
     </row>
     <row r="18" spans="2:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5">
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9">
         <v>4.3</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="9" t="s">
         <v>136</v>
       </c>
       <c r="F18" s="9" t="s">
@@ -5130,12 +5314,12 @@
       </c>
     </row>
     <row r="19" spans="2:8" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5">
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9">
         <v>4.4000000000000004</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E19" s="9" t="s">
         <v>230</v>
       </c>
       <c r="F19" s="9" t="s">
@@ -5149,12 +5333,12 @@
       </c>
     </row>
     <row r="20" spans="2:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5">
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9">
         <v>4.5</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E20" s="9" t="s">
         <v>238</v>
       </c>
       <c r="F20" s="9" t="s">
@@ -5229,7 +5413,7 @@
       </c>
     </row>
     <row r="24" spans="2:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="B24" s="21">
+      <c r="B24" s="17">
         <v>6</v>
       </c>
       <c r="C24" s="9" t="s">
@@ -5252,8 +5436,8 @@
       </c>
     </row>
     <row r="25" spans="2:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
       <c r="D25" s="9">
         <v>6.2</v>
       </c>
@@ -5271,8 +5455,8 @@
       </c>
     </row>
     <row r="26" spans="2:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
       <c r="D26" s="9">
         <v>6.3</v>
       </c>
@@ -5290,8 +5474,8 @@
       </c>
     </row>
     <row r="27" spans="2:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
       <c r="D27" s="9">
         <v>6.4</v>
       </c>
@@ -5309,36 +5493,40 @@
       </c>
     </row>
     <row r="28" spans="2:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="B28" s="5">
+      <c r="B28" s="10">
+        <v>7</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>435</v>
+      </c>
+      <c r="D28" s="11">
+        <v>7.1</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>438</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>439</v>
+      </c>
+      <c r="H28" s="11" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="B29" s="9">
         <v>8</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C29" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D28" s="5">
+      <c r="D29" s="9">
         <v>8.1</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="E29" s="9" t="s">
         <v>72</v>
-      </c>
-      <c r="F28" s="9" t="s">
-        <v>258</v>
-      </c>
-      <c r="G28" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="H28" s="9" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>74</v>
       </c>
       <c r="F29" s="9" t="s">
         <v>258</v>
@@ -5347,17 +5535,17 @@
         <v>259</v>
       </c>
       <c r="H29" s="9" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>75</v>
+        <v>261</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>74</v>
       </c>
       <c r="F30" s="9" t="s">
         <v>258</v>
@@ -5365,121 +5553,140 @@
       <c r="G30" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="H30" s="9"/>
-    </row>
-    <row r="31" spans="2:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="H30" s="9" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
       <c r="D31" s="9">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="H31" s="9"/>
+    </row>
+    <row r="32" spans="2:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9">
         <v>8.4</v>
       </c>
-      <c r="E31" s="5" t="s">
+      <c r="E32" s="9" t="s">
         <v>253</v>
       </c>
-      <c r="F31" s="9" t="s">
+      <c r="F32" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="G31" s="9" t="s">
+      <c r="G32" s="9" t="s">
         <v>260</v>
       </c>
-      <c r="H31" s="9"/>
-    </row>
-    <row r="32" spans="2:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="B32" s="11">
+      <c r="H32" s="9"/>
+    </row>
+    <row r="33" spans="2:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="B33" s="9">
         <v>9</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C33" s="9" t="s">
         <v>399</v>
       </c>
-      <c r="D32" s="11">
+      <c r="D33" s="9">
         <v>8.1</v>
       </c>
-      <c r="E32" s="11" t="s">
+      <c r="E33" s="9" t="s">
         <v>405</v>
       </c>
-      <c r="F32" s="11" t="s">
+      <c r="F33" s="9" t="s">
         <v>414</v>
       </c>
-      <c r="G32" s="11" t="s">
+      <c r="G33" s="9" t="s">
         <v>416</v>
       </c>
-      <c r="H32" s="11" t="s">
+      <c r="H33" s="9" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="33" spans="2:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="B33" s="11"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11">
+    <row r="34" spans="2:8" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9">
         <v>8.1999999999999993</v>
       </c>
-      <c r="E33" s="11" t="s">
+      <c r="E34" s="9" t="s">
         <v>406</v>
       </c>
-      <c r="F33" s="11" t="s">
+      <c r="F34" s="9" t="s">
         <v>414</v>
       </c>
-      <c r="G33" s="11" t="s">
+      <c r="G34" s="9" t="s">
         <v>416</v>
       </c>
-      <c r="H33" s="11" t="s">
+      <c r="H34" s="9" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="34" spans="2:8" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="11"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11">
+    <row r="35" spans="2:8" ht="114" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9">
         <v>8.3000000000000007</v>
       </c>
-      <c r="E34" s="11" t="s">
+      <c r="E35" s="9" t="s">
         <v>402</v>
       </c>
-      <c r="F34" s="11" t="s">
+      <c r="F35" s="9" t="s">
         <v>414</v>
       </c>
-      <c r="G34" s="11" t="s">
+      <c r="G35" s="9" t="s">
         <v>415</v>
       </c>
-      <c r="H34" s="11" t="s">
+      <c r="H35" s="9" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="35" spans="2:8" ht="114" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="11"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11">
+    <row r="36" spans="2:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9">
         <v>8.4</v>
       </c>
-      <c r="E35" s="11" t="s">
+      <c r="E36" s="9" t="s">
         <v>403</v>
       </c>
-      <c r="F35" s="11" t="s">
+      <c r="F36" s="9" t="s">
         <v>414</v>
       </c>
-      <c r="G35" s="11" t="s">
+      <c r="G36" s="9" t="s">
         <v>417</v>
       </c>
-      <c r="H35" s="11" t="s">
+      <c r="H36" s="9" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="36" spans="2:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="B36" s="11"/>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11">
+    <row r="37" spans="2:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9">
         <v>8.5</v>
       </c>
-      <c r="E36" s="11" t="s">
+      <c r="E37" s="9" t="s">
         <v>407</v>
       </c>
-      <c r="F36" s="11" t="s">
+      <c r="F37" s="9" t="s">
         <v>414</v>
       </c>
-      <c r="G36" s="11" t="s">
+      <c r="G37" s="9" t="s">
         <v>417</v>
       </c>
-      <c r="H36" s="11" t="s">
+      <c r="H37" s="9" t="s">
         <v>422</v>
       </c>
     </row>
@@ -5494,10 +5701,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BF00AFE-AD52-4AB4-8B4B-3CE4DDE5BDEE}">
-  <dimension ref="B3:G26"/>
+  <dimension ref="B3:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView topLeftCell="A23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5534,7 +5741,7 @@
       </c>
     </row>
     <row r="4" spans="2:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="B4" s="21">
+      <c r="B4" s="17">
         <v>1</v>
       </c>
       <c r="C4" s="9" t="s">
@@ -5554,7 +5761,7 @@
       </c>
     </row>
     <row r="5" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="21"/>
+      <c r="B5" s="17"/>
       <c r="C5" s="9"/>
       <c r="D5" s="9">
         <v>1.2</v>
@@ -5570,7 +5777,7 @@
       </c>
     </row>
     <row r="6" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="21"/>
+      <c r="B6" s="17"/>
       <c r="C6" s="9"/>
       <c r="D6" s="9">
         <v>1.3</v>
@@ -5586,7 +5793,7 @@
       </c>
     </row>
     <row r="7" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B7" s="21"/>
+      <c r="B7" s="17"/>
       <c r="C7" s="9"/>
       <c r="D7" s="9">
         <v>1.4</v>
@@ -5810,7 +6017,7 @@
       </c>
     </row>
     <row r="20" spans="2:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="B20" s="21">
+      <c r="B20" s="17">
         <v>6</v>
       </c>
       <c r="C20" s="9" t="s">
@@ -5830,8 +6037,8 @@
       </c>
     </row>
     <row r="21" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
       <c r="D21" s="9">
         <v>6.2</v>
       </c>
@@ -5846,8 +6053,8 @@
       </c>
     </row>
     <row r="22" spans="2:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="B22" s="21"/>
-      <c r="C22" s="21"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
       <c r="D22" s="9">
         <v>6.3</v>
       </c>
@@ -5862,8 +6069,8 @@
       </c>
     </row>
     <row r="23" spans="2:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
       <c r="D23" s="9">
         <v>6.4</v>
       </c>
@@ -5877,55 +6084,107 @@
         <v>367</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B24" s="5">
+    <row r="24" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="B24" s="10">
+        <v>7</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>435</v>
+      </c>
+      <c r="D24" s="13">
+        <v>7.1</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>441</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B25" s="10"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="13">
+        <v>7.2</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>442</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B26" s="10"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="13">
+        <v>7.4</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>436</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>445</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B27" s="5">
         <v>8</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C27" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D27" s="5">
         <v>8.1999999999999993</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="E27" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="F24" s="9" t="s">
+      <c r="F27" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="G24" s="9" t="s">
+      <c r="G27" s="9" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="25" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5">
+    <row r="28" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5">
         <v>8.3000000000000007</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="E28" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="F25" s="9" t="s">
+      <c r="F28" s="9" t="s">
         <v>290</v>
       </c>
-      <c r="G25" s="9" t="s">
+      <c r="G28" s="9" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="26" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9">
+    <row r="29" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9">
         <v>8.4</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="E29" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="F26" s="9" t="s">
+      <c r="F29" s="9" t="s">
         <v>292</v>
       </c>
-      <c r="G26" s="9" t="s">
+      <c r="G29" s="9" t="s">
         <v>293</v>
       </c>
     </row>
@@ -5939,10 +6198,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E16732A8-5A44-436B-B9F8-A4670902CDC5}">
-  <dimension ref="B2:F28"/>
+  <dimension ref="B2:F30"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6414,6 +6673,38 @@
         <v>398</v>
       </c>
     </row>
+    <row r="29" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B29" s="11">
+        <v>27</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>447</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>449</v>
+      </c>
+      <c r="F29" s="11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B30" s="11"/>
+      <c r="C30" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>450</v>
+      </c>
+      <c r="F30" s="11" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -6426,8 +6717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D749AFF6-9F01-4083-8483-60452F81DBFD}">
   <dimension ref="A1:L513"/>
   <sheetViews>
-    <sheetView topLeftCell="A507" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L477" sqref="L477"/>
+    <sheetView topLeftCell="A41" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Sprint 5 logs complete
</commit_message>
<xml_diff>
--- a/artifacts/sprint-5-logs.xlsx
+++ b/artifacts/sprint-5-logs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbens\dev\sosgame\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF99288-A4FC-4606-89E8-FBFEBAC77CB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BC9036E-079D-49BB-827A-033431086064}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7320" yWindow="75" windowWidth="21600" windowHeight="11295" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Manual Tests" sheetId="10" r:id="rId6"/>
     <sheet name="Additional Automated Tests" sheetId="11" r:id="rId7"/>
     <sheet name="Accessibility Table" sheetId="8" r:id="rId8"/>
+    <sheet name="Code Review" sheetId="12" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1007" uniqueCount="455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1063" uniqueCount="511">
   <si>
     <t>ID</t>
   </si>
@@ -1494,6 +1495,174 @@
   </si>
   <si>
     <t>Testing for the Replay class</t>
+  </si>
+  <si>
+    <t>Checklist</t>
+  </si>
+  <si>
+    <t>Checklist Item</t>
+  </si>
+  <si>
+    <t>Findings</t>
+  </si>
+  <si>
+    <t>Coding Standards</t>
+  </si>
+  <si>
+    <t>Are the naming conventions violated?</t>
+  </si>
+  <si>
+    <t>Is the ordering convention of method arguments violated?</t>
+  </si>
+  <si>
+    <t>Any comments meaningless or inconsistent with the code?</t>
+  </si>
+  <si>
+    <t>Any code block has an inconsistent formatting style?</t>
+  </si>
+  <si>
+    <t>Any indentations inconsistent?</t>
+  </si>
+  <si>
+    <t>Design Principles</t>
+  </si>
+  <si>
+    <t>Any class/method not well-modularized?</t>
+  </si>
+  <si>
+    <t>Any class with poor abstraction?</t>
+  </si>
+  <si>
+    <t>Is the visibility of any variable, method, and class inappropriate?</t>
+  </si>
+  <si>
+    <t>Is design by contract (pre/post-condition) violated?</t>
+  </si>
+  <si>
+    <t>Is the Open-Closed Principle violated?</t>
+  </si>
+  <si>
+    <t>Is the Single Responsibility Principle violated?</t>
+  </si>
+  <si>
+    <t>Code Smells</t>
+  </si>
+  <si>
+    <t>Are there magic numbers?</t>
+  </si>
+  <si>
+    <t>Are there unnecessary global / class variable?</t>
+  </si>
+  <si>
+    <t>Is there duplicate code?</t>
+  </si>
+  <si>
+    <t>Are there long methods?</t>
+  </si>
+  <si>
+    <t>Is there any long parameter list?</t>
+  </si>
+  <si>
+    <t>Is there over-complex expression?</t>
+  </si>
+  <si>
+    <t>Is there switch or if-then-else that needs to be replaced with polymorphism</t>
+  </si>
+  <si>
+    <t>Any variable or method name whose intent is unclear?</t>
+  </si>
+  <si>
+    <t>Any similar methods in different classes?</t>
+  </si>
+  <si>
+    <t>Bugs</t>
+  </si>
+  <si>
+    <t>Buggy code snippet</t>
+  </si>
+  <si>
+    <t>What is the bug?</t>
+  </si>
+  <si>
+    <t>Why is it a bug?</t>
+  </si>
+  <si>
+    <t>No, the naming conventions are not violated. The class and method names use Pascal case, where each word is capitalized. Additionally, the names accurately describe the purpose of the class or method. For example, Game is the base class for the game, and GetRow is a method that returns the row of a cell, and they both adhere to Pascal case.</t>
+  </si>
+  <si>
+    <t>No, the ordering convention of method arguments is not violated. In the code, the convention is to put any optional arguments at the end of the argument list, followed by any named arguments. For example, in the Game constructor, the optional argument recordGame is followed by the optional argument boardSize, which is followed by the optional named argument bluePlayerType.</t>
+  </si>
+  <si>
+    <t>No, the comments in the code are meaningful and consistent with the code. For example, the comment above the GameMode enumeration accurately describes the different game modes and the rules for each.</t>
+  </si>
+  <si>
+    <t>No, the classes in the code have good abstraction. For example, the Game class is an abstract base class that defines the common logic for the different types of SOS games, while the SimpleGame and GeneralGame classes are derived classes that implement the specific rules for each game mode.</t>
+  </si>
+  <si>
+    <t>No, the visibility of the variables, methods, and classes in the code is appropriate. For example, the boardSize variable in the Game class is declared as private, which means it can only be accessed from within the Game class.</t>
+  </si>
+  <si>
+    <t>Yes, the Open-Closed Principle is violated. The "Game" class contains a large number of "if" statements that determine the behavior of the game based on the game mode. This makes the class difficult to extend and modify. The class should be designed in a way that allows new game modes to be added without modifying the existing code.</t>
+  </si>
+  <si>
+    <t>Yes, the Single Responsibility Principle is violated. The "Game" class contains a large number of methods and variables that relate to different aspects of the game (e.g. game logic, player management, etc.). This makes the class difficult to understand and maintain. The class should be split into smaller, more focused classes that each have a single responsibility.</t>
+  </si>
+  <si>
+    <t>Yes, there are magic numbers in the code. For example, the "boardSize" variable is initialized with a value of 8, but this value is not explained or documented. Magic numbers should be avoided by using constants or named variables instead.</t>
+  </si>
+  <si>
+    <t>There are unnecessary global / class variables: The recordGame and boardSize variables are global variables that are not being used in the class and can be removed.</t>
+  </si>
+  <si>
+    <t>There is duplicate code: The bluePlayer and redPlayer objects are instantiated in a similar way, with the only difference being the color of the player. This can be refactored into a single method to avoid duplication.</t>
+  </si>
+  <si>
+    <t>There are long methods: The MakeMove method has a large number of lines of code and can be broken down into smaller methods to improve readability.</t>
+  </si>
+  <si>
+    <t>There is a long parameter list: The Game constructor has a long list of parameters, which can make the code difficult to read and maintain.</t>
+  </si>
+  <si>
+    <t>There is an over-complex expression: The if statement in the MakeMove method is complex and can be refactored into multiple smaller if statements for readability.</t>
+  </si>
+  <si>
+    <t>There is a switch or if-then-else that needs to be replaced with polymorphism: The bluePlayer and redPlayer objects are instantiated based on the PlayerType enum, which can be replaced with polymorphism to avoid the use of a switch statement.</t>
+  </si>
+  <si>
+    <t>Yes, the IsBoardSizeValid method name is not clear on what it does and can be renamed to something more descriptive, such as IsValidBoardSize.</t>
+  </si>
+  <si>
+    <t>The design by contract (pre/post-condition) principle is not violated in the code above. For example, the Game class's MakeMove method has a precondition that checks whether the game is over before allowing the move to be made, and it has a postcondition that updates the game state after the move is made.</t>
+  </si>
+  <si>
+    <t>The indentation is consistent in the code above. For example, the Game class's Game constructor has its arguments indented consistently, and the Player class's MakeMove method has its code blocks indented consistently.</t>
+  </si>
+  <si>
+    <t>The code block formatting is consistent in the code above. For example, all code blocks are indented using four spaces, and all lines within code blocks are indented consistently.</t>
+  </si>
+  <si>
+    <t>The Game class is well-modularized in the code above. For example, the Game class has separate methods for instantiating the players, updating the game state, and checking for a winner.</t>
+  </si>
+  <si>
+    <t>There are some similar methods in other classes. For example, the SOSEngine class also has an "EndGame" method that has different functionality from the Game.EndGame method.</t>
+  </si>
+  <si>
+    <t>The IsBoardSizeValid method checks if the board size is between 8 and 12, but it always returns true.</t>
+  </si>
+  <si>
+    <t>The IsBoardSizeValid method is intended to check if a given board size is valid, but it always returns true, so it does not actually perform this check. As a result, it will not prevent invalid board sizes from being used, which may cause unexpected behavior or errors in the program. This is a bug because the method is not fulfilling its intended purpose.</t>
+  </si>
+  <si>
+    <t>The MakeMove method uses the Debug.WriteLine method to print a message to the console.</t>
+  </si>
+  <si>
+    <t>The Debug.WriteLine method is typically used for debugging purposes. It is used to print messages to the console during development, but it should not be used in production code because it is not intended for use by end users. Instead, production code should use a logging library or other appropriate means of outputting messages to the user. Using the Debug.WriteLine method in production code may cause unexpected behavior or performance issues.</t>
+  </si>
+  <si>
+    <t>In the Game class, the GetMoves method returns a reference to the list of moves instead of a copy of the list.</t>
+  </si>
+  <si>
+    <t>This is a bug because it allows external code to modify the list of moves, which can cause errors in the game logic. It would be better to return a copy of the list so that the original list cannot be modified.</t>
   </si>
 </sst>
 </file>
@@ -1632,7 +1801,19 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="67">
+  <dxfs count="71">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -2498,130 +2679,292 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>409576</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>409575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2268934</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>1162050</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D712EE1-9754-32A7-6C22-0BEAC8BF7B71}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10191751" y="20793075"/>
+          <a:ext cx="4107258" cy="752475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>742951</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>188800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2114551</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>2057840</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C53080F-C7A4-0307-1919-9940EDD6D596}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10525126" y="22286800"/>
+          <a:ext cx="3619500" cy="1869040"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1447800</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1323975</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>876813</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C10A3D7B-2AE0-110A-4A27-5A996545569E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11229975" y="24460200"/>
+          <a:ext cx="2124075" cy="800613"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F0B81098-1FDF-4645-B026-CB44129665D9}" name="Table1" displayName="Table1" ref="C4:G13" totalsRowShown="0" headerRowDxfId="66" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F0B81098-1FDF-4645-B026-CB44129665D9}" name="Table1" displayName="Table1" ref="C4:G13" totalsRowShown="0" headerRowDxfId="70" dataDxfId="17">
   <autoFilter ref="C4:G13" xr:uid="{F0B81098-1FDF-4645-B026-CB44129665D9}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{2D6513DD-0333-4977-A611-BE7075C47F94}" name="ID" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{EA0F2575-5222-4342-B2A6-3C0DB80B27F6}" name="User Story Name" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{7B31B9E3-2E36-4F4A-87F2-E74CDAFDBBB4}" name="User Story Description" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{51BD8312-BA1E-4461-8AF6-E3CDCD58C707}" name="Priority" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{0D005556-7948-42BB-87C3-0F6B1D42DF95}" name="Estimated Effort (hours)" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{2D6513DD-0333-4977-A611-BE7075C47F94}" name="ID" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{EA0F2575-5222-4342-B2A6-3C0DB80B27F6}" name="User Story Name" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{7B31B9E3-2E36-4F4A-87F2-E74CDAFDBBB4}" name="User Story Description" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{51BD8312-BA1E-4461-8AF6-E3CDCD58C707}" name="Priority" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{0D005556-7948-42BB-87C3-0F6B1D42DF95}" name="Estimated Effort (hours)" dataDxfId="18"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{0AA3B30D-F69A-47B8-9485-B8A5F37BB8DE}" name="Table10" displayName="Table10" ref="E26:H29" totalsRowShown="0">
+  <autoFilter ref="E26:H29" xr:uid="{0AA3B30D-F69A-47B8-9485-B8A5F37BB8DE}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{4D4CA64D-2958-4503-842E-E6DCA8D38B34}" name="Bugs"/>
+    <tableColumn id="2" xr3:uid="{F9918424-45FC-4DBF-9C7F-892D0AA01C95}" name="Buggy code snippet" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{9BAC9AB1-954F-42DC-8AFF-71DAC8F79820}" name="What is the bug?" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{B8EEF6AB-E0A9-4205-986D-5516616E0668}" name="Why is it a bug?" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{412B69F0-FD73-4B7D-9BF6-3A0E4171D35B}" name="Table2" displayName="Table2" ref="B3:G38" totalsRowShown="0" dataDxfId="65">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{412B69F0-FD73-4B7D-9BF6-3A0E4171D35B}" name="Table2" displayName="Table2" ref="B3:G38" totalsRowShown="0" dataDxfId="69">
   <autoFilter ref="B3:G38" xr:uid="{412B69F0-FD73-4B7D-9BF6-3A0E4171D35B}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{702A0B1D-F950-436C-AB51-03E5AFD84C94}" name="Story ID" dataDxfId="64"/>
-    <tableColumn id="2" xr3:uid="{B7C53018-BEB1-41CB-9DD0-4289A4847403}" name="Story Name" dataDxfId="63"/>
-    <tableColumn id="3" xr3:uid="{054381AB-35EE-48FB-9EE1-95AE48FEF0FA}" name="AC ID" dataDxfId="62"/>
-    <tableColumn id="7" xr3:uid="{CF360237-B28D-40DF-928D-FC30827FC043}" name="AC Name" dataDxfId="61"/>
-    <tableColumn id="4" xr3:uid="{E3125AC9-3CDD-40AA-A1CA-0204D9A63C5C}" name="Description of Acceptance Criterion" dataDxfId="60"/>
-    <tableColumn id="5" xr3:uid="{BD32E5D0-24DE-4E60-82C8-90E318E5EA1B}" name="Status" dataDxfId="59"/>
+    <tableColumn id="1" xr3:uid="{702A0B1D-F950-436C-AB51-03E5AFD84C94}" name="Story ID" dataDxfId="68"/>
+    <tableColumn id="2" xr3:uid="{B7C53018-BEB1-41CB-9DD0-4289A4847403}" name="Story Name" dataDxfId="67"/>
+    <tableColumn id="3" xr3:uid="{054381AB-35EE-48FB-9EE1-95AE48FEF0FA}" name="AC ID" dataDxfId="66"/>
+    <tableColumn id="7" xr3:uid="{CF360237-B28D-40DF-928D-FC30827FC043}" name="AC Name" dataDxfId="65"/>
+    <tableColumn id="4" xr3:uid="{E3125AC9-3CDD-40AA-A1CA-0204D9A63C5C}" name="Description of Acceptance Criterion" dataDxfId="64"/>
+    <tableColumn id="5" xr3:uid="{BD32E5D0-24DE-4E60-82C8-90E318E5EA1B}" name="Status" dataDxfId="63"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D36D6B9B-3977-42E1-9D3A-2AD19D09F63F}" name="Table3" displayName="Table3" ref="B4:E28" totalsRowCount="1" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D36D6B9B-3977-42E1-9D3A-2AD19D09F63F}" name="Table3" displayName="Table3" ref="B4:E28" totalsRowCount="1" dataDxfId="12">
   <autoFilter ref="B4:E27" xr:uid="{D36D6B9B-3977-42E1-9D3A-2AD19D09F63F}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:E27">
     <sortCondition ref="C5:C27"/>
     <sortCondition descending="1" ref="E5:E27"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{DB279ACC-EE7F-4F69-9CDF-D6557C3D4B5F}" name="Source Code file Name" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{AD6AFAE9-FED0-4CE4-8020-D0B3CA4EBBA2}" name="Production code or test code?" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{FDFB077A-2AFB-452D-8B38-C052AFA8880B}" name="Notes" totalsRowLabel="Total" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{9C1EC1B0-7F07-45F8-AACD-2593D2FB6FC3}" name="# Lines of Code" totalsRowFunction="sum" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{DB279ACC-EE7F-4F69-9CDF-D6557C3D4B5F}" name="Source Code file Name" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{AD6AFAE9-FED0-4CE4-8020-D0B3CA4EBBA2}" name="Production code or test code?" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{FDFB077A-2AFB-452D-8B38-C052AFA8880B}" name="Notes" totalsRowLabel="Total" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{9C1EC1B0-7F07-45F8-AACD-2593D2FB6FC3}" name="# Lines of Code" totalsRowFunction="sum" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{8613F438-F257-4CB7-8127-41336443AD8E}" name="Table5" displayName="Table5" ref="B4:I35" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{8613F438-F257-4CB7-8127-41336443AD8E}" name="Table5" displayName="Table5" ref="B4:I35" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61">
   <autoFilter ref="B4:I35" xr:uid="{8613F438-F257-4CB7-8127-41336443AD8E}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{FA37DF55-838D-4C91-A069-B4ADFBB114FF}" name="Story ID" dataDxfId="56"/>
-    <tableColumn id="7" xr3:uid="{B29593B2-9E50-4429-B73E-C267894CE53F}" name="Story Name" dataDxfId="55"/>
-    <tableColumn id="2" xr3:uid="{92144E97-78C1-4013-A5DC-A103AC987D08}" name="AC  ID" dataDxfId="54"/>
-    <tableColumn id="8" xr3:uid="{D34169B1-9605-4002-A5FC-55DBEC95591D}" name="AC Name" dataDxfId="53"/>
-    <tableColumn id="3" xr3:uid="{988A7BC5-9B7F-4EF4-9743-8B43044CA88C}" name="Classes" dataDxfId="52"/>
-    <tableColumn id="4" xr3:uid="{6962998B-BD75-44D2-8DE4-A3B7232E7D55}" name="Method Name(s) " dataDxfId="51"/>
-    <tableColumn id="5" xr3:uid="{8D2432C4-71E4-445C-BF93-B65E87280890}" name="Status" dataDxfId="50"/>
-    <tableColumn id="6" xr3:uid="{1E10CD18-6EE0-4C57-A597-745A6F075070}" name="Notes (optional)" dataDxfId="49"/>
+    <tableColumn id="1" xr3:uid="{FA37DF55-838D-4C91-A069-B4ADFBB114FF}" name="Story ID" dataDxfId="60"/>
+    <tableColumn id="7" xr3:uid="{B29593B2-9E50-4429-B73E-C267894CE53F}" name="Story Name" dataDxfId="59"/>
+    <tableColumn id="2" xr3:uid="{92144E97-78C1-4013-A5DC-A103AC987D08}" name="AC  ID" dataDxfId="58"/>
+    <tableColumn id="8" xr3:uid="{D34169B1-9605-4002-A5FC-55DBEC95591D}" name="AC Name" dataDxfId="57"/>
+    <tableColumn id="3" xr3:uid="{988A7BC5-9B7F-4EF4-9743-8B43044CA88C}" name="Classes" dataDxfId="56"/>
+    <tableColumn id="4" xr3:uid="{6962998B-BD75-44D2-8DE4-A3B7232E7D55}" name="Method Name(s) " dataDxfId="55"/>
+    <tableColumn id="5" xr3:uid="{8D2432C4-71E4-445C-BF93-B65E87280890}" name="Status" dataDxfId="54"/>
+    <tableColumn id="6" xr3:uid="{1E10CD18-6EE0-4C57-A597-745A6F075070}" name="Notes (optional)" dataDxfId="53"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{AFC835DF-2809-4ADA-8933-35F8B41412B7}" name="Table6" displayName="Table6" ref="B3:H37" totalsRowShown="0" headerRowDxfId="48" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{AFC835DF-2809-4ADA-8933-35F8B41412B7}" name="Table6" displayName="Table6" ref="B3:H37" totalsRowShown="0" headerRowDxfId="52" dataDxfId="4">
   <autoFilter ref="B3:H37" xr:uid="{AFC835DF-2809-4ADA-8933-35F8B41412B7}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{4D464094-4CAA-4F0A-8155-1005A5221EA7}" name="User Story ID" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{DFFD886B-21F5-4EE4-B1E5-B9C3CA981393}" name="User Story Name" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{588A5FF9-87E4-4232-A109-F00AE6EAB7C9}" name="AC ID" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{A723F0C9-F396-4182-A5DB-A36687ECC464}" name="AC Name" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{04A7B299-94AB-4FB7-8A08-822F463E676E}" name="Classes " dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{263669AA-535C-4DA8-9C9A-A153A480F553}" name="Methods" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{9CFC3D83-A897-493C-A6B2-E4D0BA51E596}" name="Description" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{4D464094-4CAA-4F0A-8155-1005A5221EA7}" name="User Story ID" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{DFFD886B-21F5-4EE4-B1E5-B9C3CA981393}" name="User Story Name" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{588A5FF9-87E4-4232-A109-F00AE6EAB7C9}" name="AC ID" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{A723F0C9-F396-4182-A5DB-A36687ECC464}" name="AC Name" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{04A7B299-94AB-4FB7-8A08-822F463E676E}" name="Classes " dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{263669AA-535C-4DA8-9C9A-A153A480F553}" name="Methods" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{9CFC3D83-A897-493C-A6B2-E4D0BA51E596}" name="Description" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{A6E1AD56-1E7E-4845-A6DC-51274101CF0C}" name="Table69" displayName="Table69" ref="B3:G29" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{A6E1AD56-1E7E-4845-A6DC-51274101CF0C}" name="Table69" displayName="Table69" ref="B3:G29" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
   <autoFilter ref="B3:G29" xr:uid="{AFC835DF-2809-4ADA-8933-35F8B41412B7}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{301EF044-7DF2-4C9B-84A0-556EDC81E926}" name="User Story ID" dataDxfId="45"/>
-    <tableColumn id="6" xr3:uid="{C53176BB-A112-4BC9-B43C-A9B819FD40BE}" name="User Story Name" dataDxfId="44"/>
-    <tableColumn id="2" xr3:uid="{75701814-A8A2-49F2-9634-F7BCE794B67D}" name="AC ID" dataDxfId="43"/>
-    <tableColumn id="7" xr3:uid="{DB2FE0C2-4D4A-4FA4-AD4F-2F9ACE0E2772}" name="AC Name" dataDxfId="42"/>
-    <tableColumn id="4" xr3:uid="{5FE8A6D0-B4D1-471F-9956-459A848C1C0F}" name="Test Case Input" dataDxfId="41"/>
-    <tableColumn id="5" xr3:uid="{C8A349CF-C07B-44C4-B8D0-DD604B478305}" name="Test Oracle" dataDxfId="40"/>
+    <tableColumn id="1" xr3:uid="{301EF044-7DF2-4C9B-84A0-556EDC81E926}" name="User Story ID" dataDxfId="49"/>
+    <tableColumn id="6" xr3:uid="{C53176BB-A112-4BC9-B43C-A9B819FD40BE}" name="User Story Name" dataDxfId="48"/>
+    <tableColumn id="2" xr3:uid="{75701814-A8A2-49F2-9634-F7BCE794B67D}" name="AC ID" dataDxfId="47"/>
+    <tableColumn id="7" xr3:uid="{DB2FE0C2-4D4A-4FA4-AD4F-2F9ACE0E2772}" name="AC Name" dataDxfId="46"/>
+    <tableColumn id="4" xr3:uid="{5FE8A6D0-B4D1-471F-9956-459A848C1C0F}" name="Test Case Input" dataDxfId="45"/>
+    <tableColumn id="5" xr3:uid="{C8A349CF-C07B-44C4-B8D0-DD604B478305}" name="Test Oracle" dataDxfId="44"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{0F699053-0EA0-422C-84BA-6343D3283560}" name="Table9" displayName="Table9" ref="B2:F30" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{0F699053-0EA0-422C-84BA-6343D3283560}" name="Table9" displayName="Table9" ref="B2:F30" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
   <autoFilter ref="B2:F30" xr:uid="{0F699053-0EA0-422C-84BA-6343D3283560}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{7EE5C09C-96A5-4FC0-A9B8-78BA2D61269E}" name="Number" dataDxfId="37"/>
-    <tableColumn id="2" xr3:uid="{B9AA6030-119E-443A-BB87-750EA97ECF8C}" name="Production Code Class.Method" dataDxfId="36"/>
-    <tableColumn id="5" xr3:uid="{49E194BC-903C-4C2D-AF6F-5DBC479ACEC9}" name="Test Code Class.Method" dataDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{9D11DD5C-4AE4-4A5E-8750-0E12B5A106FA}" name="Test Input" dataDxfId="34"/>
-    <tableColumn id="4" xr3:uid="{8C3EBF53-C850-403C-B499-DB556E2F1A8B}" name="Expected Result" dataDxfId="33"/>
+    <tableColumn id="1" xr3:uid="{7EE5C09C-96A5-4FC0-A9B8-78BA2D61269E}" name="Number" dataDxfId="41"/>
+    <tableColumn id="2" xr3:uid="{B9AA6030-119E-443A-BB87-750EA97ECF8C}" name="Production Code Class.Method" dataDxfId="40"/>
+    <tableColumn id="5" xr3:uid="{49E194BC-903C-4C2D-AF6F-5DBC479ACEC9}" name="Test Code Class.Method" dataDxfId="39"/>
+    <tableColumn id="3" xr3:uid="{9D11DD5C-4AE4-4A5E-8750-0E12B5A106FA}" name="Test Input" dataDxfId="38"/>
+    <tableColumn id="4" xr3:uid="{8C3EBF53-C850-403C-B499-DB556E2F1A8B}" name="Expected Result" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{69FD6488-0717-4BB3-A73F-84BDA7E946E5}" name="Table4" displayName="Table4" ref="A1:L513" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{69FD6488-0717-4BB3-A73F-84BDA7E946E5}" name="Table4" displayName="Table4" ref="A1:L513" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
   <autoFilter ref="A1:L513" xr:uid="{69FD6488-0717-4BB3-A73F-84BDA7E946E5}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{4EEA4C52-25A8-4AC1-AB64-130F1061C5C0}" name="Control Name" dataDxfId="30"/>
-    <tableColumn id="2" xr3:uid="{528C3ED4-7A70-4ADC-A6E5-12A55306EB86}" name="Control A" dataDxfId="29"/>
-    <tableColumn id="3" xr3:uid="{5A820990-15C8-451A-AA81-A4FDEEF27F37}" name="Control B" dataDxfId="28"/>
-    <tableColumn id="4" xr3:uid="{90491295-6B5C-44D5-9DBA-7086E88AC0F9}" name="Control C" dataDxfId="27"/>
-    <tableColumn id="5" xr3:uid="{1C3B15D1-EB06-4A22-B868-6BE0E2AA4E0D}" name="Control D" dataDxfId="26"/>
-    <tableColumn id="6" xr3:uid="{EB1C9048-B008-4402-8AFC-D23757742E6F}" name="In Replay" dataDxfId="25"/>
-    <tableColumn id="7" xr3:uid="{B62C2260-705C-4FA8-AAD7-D8CDD79F071C}" name="In Game" dataDxfId="24"/>
-    <tableColumn id="12" xr3:uid="{7DBAE433-F5CB-4355-AA42-DF22721518A4}" name="Is Red Turn" dataDxfId="23"/>
-    <tableColumn id="8" xr3:uid="{E7051258-A7C3-4770-BF85-6A7E897040FA}" name="Is Blue Computer" dataDxfId="22"/>
-    <tableColumn id="9" xr3:uid="{672057EC-F845-40E7-A956-72F68FFFCD00}" name="Is Red Computer" dataDxfId="21"/>
-    <tableColumn id="10" xr3:uid="{43FEA681-4DBD-4D98-B67C-A034045E34F1}" name="Is Accessible" dataDxfId="20"/>
-    <tableColumn id="11" xr3:uid="{72EB1685-1373-450C-B014-35BFBA34CCA1}" name="Notes" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{4EEA4C52-25A8-4AC1-AB64-130F1061C5C0}" name="Control Name" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{528C3ED4-7A70-4ADC-A6E5-12A55306EB86}" name="Control A" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{5A820990-15C8-451A-AA81-A4FDEEF27F37}" name="Control B" dataDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{90491295-6B5C-44D5-9DBA-7086E88AC0F9}" name="Control C" dataDxfId="31"/>
+    <tableColumn id="5" xr3:uid="{1C3B15D1-EB06-4A22-B868-6BE0E2AA4E0D}" name="Control D" dataDxfId="30"/>
+    <tableColumn id="6" xr3:uid="{EB1C9048-B008-4402-8AFC-D23757742E6F}" name="In Replay" dataDxfId="29"/>
+    <tableColumn id="7" xr3:uid="{B62C2260-705C-4FA8-AAD7-D8CDD79F071C}" name="In Game" dataDxfId="28"/>
+    <tableColumn id="12" xr3:uid="{7DBAE433-F5CB-4355-AA42-DF22721518A4}" name="Is Red Turn" dataDxfId="27"/>
+    <tableColumn id="8" xr3:uid="{E7051258-A7C3-4770-BF85-6A7E897040FA}" name="Is Blue Computer" dataDxfId="26"/>
+    <tableColumn id="9" xr3:uid="{672057EC-F845-40E7-A956-72F68FFFCD00}" name="Is Red Computer" dataDxfId="25"/>
+    <tableColumn id="10" xr3:uid="{43FEA681-4DBD-4D98-B67C-A034045E34F1}" name="Is Accessible" dataDxfId="24"/>
+    <tableColumn id="11" xr3:uid="{72EB1685-1373-450C-B014-35BFBA34CCA1}" name="Notes" dataDxfId="23"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{C480FF4E-0571-48BF-9270-CB9840704F1F}" name="Table7" displayName="Table7" ref="B2:D22" totalsRowShown="0">
+  <autoFilter ref="B2:D22" xr:uid="{C480FF4E-0571-48BF-9270-CB9840704F1F}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{D16B1B45-3117-445D-B6B7-D8032E4CB16E}" name="Checklist"/>
+    <tableColumn id="2" xr3:uid="{580CC1A5-67F8-41C1-835E-C40FE72F92AF}" name="Checklist Item"/>
+    <tableColumn id="3" xr3:uid="{609A034E-FB49-4077-9A8C-A25C8C3A4153}" name="Findings" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2892,8 +3235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C2:G13"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3099,8 +3442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DCE3E03-8907-42B0-9BAE-1522C8D2D080}">
   <dimension ref="B2:H49"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29:E29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3842,8 +4185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1EAF2C1-6E6A-4763-B1B8-87DF226FCFDA}">
   <dimension ref="B4:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24702,4 +25045,254 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3640183C-6F9D-4C93-AC61-8429EEA4D33E}">
+  <dimension ref="B2:H29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26:H29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="69.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="33.7109375" customWidth="1"/>
+    <col min="6" max="6" width="42.42578125" customWidth="1"/>
+    <col min="7" max="7" width="31.7109375" customWidth="1"/>
+    <col min="8" max="8" width="41" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>455</v>
+      </c>
+      <c r="C2" t="s">
+        <v>456</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>458</v>
+      </c>
+      <c r="C3" t="s">
+        <v>459</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>460</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>461</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>462</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>463</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>464</v>
+      </c>
+      <c r="C8" t="s">
+        <v>465</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>466</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>467</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>468</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>469</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>470</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>471</v>
+      </c>
+      <c r="C14" t="s">
+        <v>472</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>473</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>474</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="17" spans="3:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>475</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="18" spans="3:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>476</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="19" spans="3:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>477</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="20" spans="3:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>478</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="21" spans="3:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>479</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="22" spans="3:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>480</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="26" spans="3:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>481</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="H26" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="27" spans="3:8" ht="135" x14ac:dyDescent="0.25">
+      <c r="F27" s="1"/>
+      <c r="G27" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="28" spans="3:8" ht="180" x14ac:dyDescent="0.25">
+      <c r="F28" s="1"/>
+      <c r="G28" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="29" spans="3:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="F29" s="1"/>
+      <c r="G29" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>510</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>